<commit_message>
02/09 avance prog concilia auto 2h
</commit_message>
<xml_diff>
--- a/SGLibrary_COM/archivo_ejemplo/analisis_archivos_tarjetas.xlsx
+++ b/SGLibrary_COM/archivo_ejemplo/analisis_archivos_tarjetas.xlsx
@@ -463,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M35"/>
+  <dimension ref="B2:M36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,80 +599,81 @@
         <v>14</v>
       </c>
     </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <v>6</v>
+      </c>
+      <c r="J6">
+        <v>7</v>
+      </c>
+      <c r="K6">
+        <v>8</v>
+      </c>
+      <c r="L6">
+        <v>9</v>
+      </c>
+      <c r="M6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="K7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="L7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="M7" s="3" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7">
-        <v>20747964</v>
-      </c>
-      <c r="D7" s="2">
-        <v>42599</v>
-      </c>
-      <c r="E7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7">
-        <v>3624</v>
-      </c>
-      <c r="G7">
-        <v>6</v>
-      </c>
-      <c r="H7" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J7" t="s">
-        <v>29</v>
-      </c>
-      <c r="K7" t="s">
-        <v>30</v>
-      </c>
-      <c r="L7" s="2">
-        <v>42625</v>
-      </c>
-      <c r="M7">
-        <v>67961</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
@@ -689,10 +690,10 @@
         <v>26</v>
       </c>
       <c r="F8">
-        <v>4075</v>
+        <v>3624</v>
       </c>
       <c r="G8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H8" t="s">
         <v>27</v>
@@ -701,10 +702,10 @@
         <v>28</v>
       </c>
       <c r="J8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L8" s="2">
         <v>42625</v>
@@ -713,154 +714,181 @@
         <v>67961</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C11" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>33</v>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9">
+        <v>20747964</v>
+      </c>
+      <c r="D9" s="2">
+        <v>42599</v>
+      </c>
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9">
+        <v>4075</v>
+      </c>
+      <c r="G9">
+        <v>7</v>
+      </c>
+      <c r="H9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" t="s">
+        <v>31</v>
+      </c>
+      <c r="K9" t="s">
+        <v>32</v>
+      </c>
+      <c r="L9" s="2">
+        <v>42625</v>
+      </c>
+      <c r="M9">
+        <v>67961</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C12" s="3" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C13" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I13" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C14" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="G14" s="3"/>
       <c r="H14" s="3" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C15" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C16" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="I17" s="3" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C18" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I18" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C19" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C20" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C21" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C23" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
-        <v>35</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E29" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="30" spans="3:9" x14ac:dyDescent="0.25">
@@ -868,7 +896,7 @@
         <v>35</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="E30" t="s">
         <v>36</v>
@@ -879,7 +907,7 @@
         <v>35</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E31" t="s">
         <v>36</v>
@@ -890,7 +918,7 @@
         <v>35</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E32" t="s">
         <v>36</v>
@@ -901,7 +929,7 @@
         <v>35</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E33" t="s">
         <v>36</v>
@@ -912,7 +940,7 @@
         <v>35</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E34" t="s">
         <v>36</v>
@@ -923,9 +951,20 @@
         <v>35</v>
       </c>
       <c r="D35" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>35</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E36" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>